<commit_message>
add xlsx for parser
</commit_message>
<xml_diff>
--- a/components/document/parser/xlsx/testdata/location.xlsx
+++ b/components/document/parser/xlsx/testdata/location.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20723\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4660D2AB-0118-4832-84A9-6ED25809A425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4A051-B614-4477-A9D0-0017F129AF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4524" yWindow="1140" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>省</t>
   </si>
@@ -55,6 +57,22 @@
   </si>
   <si>
     <t>龙亭区</t>
+  </si>
+  <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>good</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -461,11 +479,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4702C1A9-1183-4CDD-9667-74E8F22375AD}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0361B-B6B0-4B3E-97AD-240CB1A3354B}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat:add parser for xlsx
</commit_message>
<xml_diff>
--- a/components/document/parser/xlsx/testdata/location.xlsx
+++ b/components/document/parser/xlsx/testdata/location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20723\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4A051-B614-4477-A9D0-0017F129AF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727E2B5B-75A7-448D-A613-465C641497BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="1140" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4524" yWindow="1140" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -27,37 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
-  <si>
-    <t>省</t>
-  </si>
-  <si>
-    <t>市</t>
-  </si>
-  <si>
-    <t>县（区）</t>
-  </si>
-  <si>
-    <t>河南省</t>
-  </si>
-  <si>
-    <t>郑州市</t>
-  </si>
-  <si>
-    <t>新密市</t>
-  </si>
-  <si>
-    <t>新郑市</t>
-  </si>
-  <si>
-    <t>登封市</t>
-  </si>
-  <si>
-    <t>开封市</t>
-  </si>
-  <si>
-    <t>龙亭区</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>hello</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +42,42 @@
   </si>
   <si>
     <t>game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年龄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王丽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,29 +486,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4702C1A9-1183-4CDD-9667-74E8F22375AD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="6">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -512,29 +562,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="6">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -544,73 +638,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0361B-B6B0-4B3E-97AD-240CB1A3354B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>